<commit_message>
Add test import data, for case 1 record.
</commit_message>
<xml_diff>
--- a/test_import/Order.xlsx
+++ b/test_import/Order.xlsx
@@ -8,14 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Order_2015-08-03_110007" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Order_2015-08-03_110007'!$A$1:$AW$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'order_2015-08-03_110007'!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'order_2015-08-03_110007'!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'order_2015-08-03_110007'!#ref!</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
@@ -490,21 +484,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8663967611336"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +644,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>4358272</v>
       </c>
@@ -804,9 +792,8 @@
       <c r="AW2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="3" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>4357474</v>
       </c>
@@ -954,9 +941,8 @@
       <c r="AW3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>4435660</v>
       </c>
@@ -1104,9 +1090,8 @@
       <c r="AW4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="4" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>4435659</v>
       </c>
@@ -1254,9 +1239,8 @@
       <c r="AW5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="5" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>4345076</v>
       </c>
@@ -1404,9 +1388,8 @@
       <c r="AW6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="5" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>4345075</v>
       </c>
@@ -1554,9 +1537,8 @@
       <c r="AW7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>4345074</v>
       </c>
@@ -1704,9 +1686,8 @@
       <c r="AW8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="5" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>4345073</v>
       </c>
@@ -1854,15 +1835,14 @@
       <c r="AW9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AMJ9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>